<commit_message>
added the changes to forecast with 6D timeseries
</commit_message>
<xml_diff>
--- a/code/imputationExperiment/Experiment_Excel.xlsx
+++ b/code/imputationExperiment/Experiment_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maarten\Desktop\Afstuderen\thesis_stock_prediction_repo\code\imputationExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5D5F81-CBB9-4432-86B3-4FD4651C8533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B88D04D-51FE-417F-8F60-0D9A287CF909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="0" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="4" xr2:uid="{C28E17DC-67F8-4148-B879-84FD1B20D75B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{C28E17DC-67F8-4148-B879-84FD1B20D75B}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment optimization" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="344">
   <si>
     <t>Data</t>
   </si>
@@ -607,9 +607,6 @@
     <t>IM-15</t>
   </si>
   <si>
-    <t>Wextrapolatecubic</t>
-  </si>
-  <si>
     <t>IM-16</t>
   </si>
   <si>
@@ -622,9 +619,6 @@
     <t>IM-18</t>
   </si>
   <si>
-    <t>Wextrapolatelinear</t>
-  </si>
-  <si>
     <t>IM-19</t>
   </si>
   <si>
@@ -764,6 +758,318 @@
   </si>
   <si>
     <t>IM-64</t>
+  </si>
+  <si>
+    <t>IM-72</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>IM-73</t>
+  </si>
+  <si>
+    <t>IM-74</t>
+  </si>
+  <si>
+    <t>IM-75</t>
+  </si>
+  <si>
+    <t>IM-76</t>
+  </si>
+  <si>
+    <t>IM-77</t>
+  </si>
+  <si>
+    <t>IM-78</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>IM-79</t>
+  </si>
+  <si>
+    <t>IM-80</t>
+  </si>
+  <si>
+    <t>IM-81</t>
+  </si>
+  <si>
+    <t>IM-82</t>
+  </si>
+  <si>
+    <t>IM-83</t>
+  </si>
+  <si>
+    <t>IM-84</t>
+  </si>
+  <si>
+    <t>IM-85</t>
+  </si>
+  <si>
+    <t>IM-86</t>
+  </si>
+  <si>
+    <t>IM-87</t>
+  </si>
+  <si>
+    <t>IM-88</t>
+  </si>
+  <si>
+    <t>IM-89</t>
+  </si>
+  <si>
+    <t>IM-90</t>
+  </si>
+  <si>
+    <t>IM-91</t>
+  </si>
+  <si>
+    <t>IM-92</t>
+  </si>
+  <si>
+    <t>IM-93</t>
+  </si>
+  <si>
+    <t>IM-94</t>
+  </si>
+  <si>
+    <t>IM-95</t>
+  </si>
+  <si>
+    <t>IM-96</t>
+  </si>
+  <si>
+    <t>IM-97</t>
+  </si>
+  <si>
+    <t>IM-98</t>
+  </si>
+  <si>
+    <t>IM-99</t>
+  </si>
+  <si>
+    <t>IM-171</t>
+  </si>
+  <si>
+    <t>IM-170</t>
+  </si>
+  <si>
+    <t>IM-169</t>
+  </si>
+  <si>
+    <t>IM-168</t>
+  </si>
+  <si>
+    <t>IM-167</t>
+  </si>
+  <si>
+    <t>IM-166</t>
+  </si>
+  <si>
+    <t>IM-165</t>
+  </si>
+  <si>
+    <t>IM-164</t>
+  </si>
+  <si>
+    <t>IM-163</t>
+  </si>
+  <si>
+    <t>IM-162</t>
+  </si>
+  <si>
+    <t>IM-161</t>
+  </si>
+  <si>
+    <t>IM-160</t>
+  </si>
+  <si>
+    <t>IM-159</t>
+  </si>
+  <si>
+    <t>IM-158</t>
+  </si>
+  <si>
+    <t>IM-157</t>
+  </si>
+  <si>
+    <t>IM-156</t>
+  </si>
+  <si>
+    <t>IM-155</t>
+  </si>
+  <si>
+    <t>IM-154</t>
+  </si>
+  <si>
+    <t>IM-153</t>
+  </si>
+  <si>
+    <t>IM-152</t>
+  </si>
+  <si>
+    <t>IM-151</t>
+  </si>
+  <si>
+    <t>IM-150</t>
+  </si>
+  <si>
+    <t>IM-149</t>
+  </si>
+  <si>
+    <t>IM-148</t>
+  </si>
+  <si>
+    <t>IM-147</t>
+  </si>
+  <si>
+    <t>IM-146</t>
+  </si>
+  <si>
+    <t>IM-145</t>
+  </si>
+  <si>
+    <t>IM-144</t>
+  </si>
+  <si>
+    <t>IM-143</t>
+  </si>
+  <si>
+    <t>IM-142</t>
+  </si>
+  <si>
+    <t>IM-141</t>
+  </si>
+  <si>
+    <t>IM-140</t>
+  </si>
+  <si>
+    <t>IM-139</t>
+  </si>
+  <si>
+    <t>IM-138</t>
+  </si>
+  <si>
+    <t>IM-137</t>
+  </si>
+  <si>
+    <t>IM-136</t>
+  </si>
+  <si>
+    <t>IM-135</t>
+  </si>
+  <si>
+    <t>IM-134</t>
+  </si>
+  <si>
+    <t>IM-133</t>
+  </si>
+  <si>
+    <t>IM-132</t>
+  </si>
+  <si>
+    <t>IM-131</t>
+  </si>
+  <si>
+    <t>IM-130</t>
+  </si>
+  <si>
+    <t>IM-129</t>
+  </si>
+  <si>
+    <t>IM-128</t>
+  </si>
+  <si>
+    <t>IM-127</t>
+  </si>
+  <si>
+    <t>IM-126</t>
+  </si>
+  <si>
+    <t>IM-125</t>
+  </si>
+  <si>
+    <t>IM-124</t>
+  </si>
+  <si>
+    <t>IM-123</t>
+  </si>
+  <si>
+    <t>IM-122</t>
+  </si>
+  <si>
+    <t>IM-121</t>
+  </si>
+  <si>
+    <t>IM-120</t>
+  </si>
+  <si>
+    <t>IM-119</t>
+  </si>
+  <si>
+    <t>IM-118</t>
+  </si>
+  <si>
+    <t>IM-117</t>
+  </si>
+  <si>
+    <t>IM-116</t>
+  </si>
+  <si>
+    <t>IM-115</t>
+  </si>
+  <si>
+    <t>IM-114</t>
+  </si>
+  <si>
+    <t>IM-113</t>
+  </si>
+  <si>
+    <t>IM-112</t>
+  </si>
+  <si>
+    <t>IM-111</t>
+  </si>
+  <si>
+    <t>IM-110</t>
+  </si>
+  <si>
+    <t>IM-109</t>
+  </si>
+  <si>
+    <t>IM-108</t>
+  </si>
+  <si>
+    <t>IM-107</t>
+  </si>
+  <si>
+    <t>IM-106</t>
+  </si>
+  <si>
+    <t>IM-105</t>
+  </si>
+  <si>
+    <t>IM-104</t>
+  </si>
+  <si>
+    <t>IM-103</t>
+  </si>
+  <si>
+    <t>IM-102</t>
+  </si>
+  <si>
+    <t>IM-101</t>
+  </si>
+  <si>
+    <t>IM-100</t>
+  </si>
+  <si>
+    <t>cubic</t>
+  </si>
+  <si>
+    <t>linear</t>
   </si>
 </sst>
 </file>
@@ -6480,10 +6786,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B822772-3EEA-483C-8175-4ED0E2CC6085}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6524,7 +6830,7 @@
         <v>0.33</v>
       </c>
       <c r="D2" s="64" t="s">
-        <v>189</v>
+        <v>342</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -6535,7 +6841,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
         <v>187</v>
@@ -6544,7 +6850,7 @@
         <v>0.33</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -6555,7 +6861,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
         <v>187</v>
@@ -6564,7 +6870,7 @@
         <v>0.33</v>
       </c>
       <c r="D4" s="64" t="s">
-        <v>194</v>
+        <v>343</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -6575,7 +6881,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B5" t="s">
         <v>187</v>
@@ -6595,7 +6901,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
         <v>187</v>
@@ -6604,7 +6910,7 @@
         <v>0.33</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -6615,7 +6921,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
         <v>187</v>
@@ -6624,7 +6930,7 @@
         <v>0.33</v>
       </c>
       <c r="D7" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6635,7 +6941,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s">
         <v>187</v>
@@ -6644,7 +6950,7 @@
         <v>0.33</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>194</v>
+        <v>343</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -6655,7 +6961,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B9" t="s">
         <v>187</v>
@@ -6664,7 +6970,7 @@
         <v>0.33</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>189</v>
+        <v>342</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -6675,7 +6981,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B10" t="s">
         <v>187</v>
@@ -6684,7 +6990,7 @@
         <v>0.33</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -6695,7 +7001,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B11" t="s">
         <v>187</v>
@@ -6715,7 +7021,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B12" t="s">
         <v>187</v>
@@ -6724,7 +7030,7 @@
         <v>0.33</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -6735,7 +7041,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B13" t="s">
         <v>187</v>
@@ -6744,7 +7050,7 @@
         <v>0.33</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>194</v>
+        <v>343</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -6755,7 +7061,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B14" t="s">
         <v>187</v>
@@ -6764,7 +7070,7 @@
         <v>0.33</v>
       </c>
       <c r="D14" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -6775,7 +7081,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B15" t="s">
         <v>187</v>
@@ -6784,7 +7090,7 @@
         <v>0.33</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>189</v>
+        <v>342</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -6795,7 +7101,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B16" t="s">
         <v>187</v>
@@ -6815,7 +7121,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B17" t="s">
         <v>187</v>
@@ -6824,7 +7130,7 @@
         <v>0.33</v>
       </c>
       <c r="D17" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -6835,7 +7141,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B18" t="s">
         <v>187</v>
@@ -6844,7 +7150,7 @@
         <v>0.33</v>
       </c>
       <c r="D18" s="64" t="s">
-        <v>194</v>
+        <v>343</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -6855,7 +7161,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B19" t="s">
         <v>187</v>
@@ -6864,7 +7170,7 @@
         <v>0.33</v>
       </c>
       <c r="D19" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -6875,7 +7181,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B20" t="s">
         <v>187</v>
@@ -6884,7 +7190,7 @@
         <v>0.33</v>
       </c>
       <c r="D20" s="64" t="s">
-        <v>189</v>
+        <v>342</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -6895,7 +7201,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B21" t="s">
         <v>187</v>
@@ -6915,7 +7221,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B22" t="s">
         <v>187</v>
@@ -6924,7 +7230,7 @@
         <v>0.33</v>
       </c>
       <c r="D22" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -6935,7 +7241,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B23" t="s">
         <v>187</v>
@@ -6944,7 +7250,7 @@
         <v>0.33</v>
       </c>
       <c r="D23" s="64" t="s">
-        <v>194</v>
+        <v>343</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -6955,7 +7261,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B24" t="s">
         <v>187</v>
@@ -6964,7 +7270,7 @@
         <v>0.33</v>
       </c>
       <c r="D24" s="64" t="s">
-        <v>189</v>
+        <v>342</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -6975,7 +7281,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B25" t="s">
         <v>187</v>
@@ -6984,7 +7290,7 @@
         <v>0.33</v>
       </c>
       <c r="D25" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -6995,7 +7301,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B26" t="s">
         <v>187</v>
@@ -7015,7 +7321,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B27" t="s">
         <v>187</v>
@@ -7024,7 +7330,7 @@
         <v>0.9</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -7035,7 +7341,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B28" t="s">
         <v>187</v>
@@ -7044,7 +7350,7 @@
         <v>0.9</v>
       </c>
       <c r="D28" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -7055,7 +7361,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B29" t="s">
         <v>187</v>
@@ -7064,7 +7370,7 @@
         <v>0.9</v>
       </c>
       <c r="D29" s="64" t="s">
-        <v>189</v>
+        <v>342</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -7075,7 +7381,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B30" t="s">
         <v>187</v>
@@ -7084,7 +7390,7 @@
         <v>0.9</v>
       </c>
       <c r="D30" s="64" t="s">
-        <v>194</v>
+        <v>343</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -7095,7 +7401,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B31" t="s">
         <v>187</v>
@@ -7115,7 +7421,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B32" t="s">
         <v>187</v>
@@ -7124,7 +7430,7 @@
         <v>0.9</v>
       </c>
       <c r="D32" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -7135,7 +7441,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B33" t="s">
         <v>187</v>
@@ -7144,7 +7450,7 @@
         <v>0.9</v>
       </c>
       <c r="D33" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -7155,7 +7461,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B34" t="s">
         <v>187</v>
@@ -7175,7 +7481,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B35" t="s">
         <v>187</v>
@@ -7184,7 +7490,7 @@
         <v>0.9</v>
       </c>
       <c r="D35" s="64" t="s">
-        <v>189</v>
+        <v>342</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -7195,7 +7501,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B36" t="s">
         <v>187</v>
@@ -7204,7 +7510,7 @@
         <v>0.9</v>
       </c>
       <c r="D36" s="64" t="s">
-        <v>194</v>
+        <v>343</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -7215,7 +7521,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B37" t="s">
         <v>187</v>
@@ -7224,7 +7530,7 @@
         <v>0.9</v>
       </c>
       <c r="D37" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -7235,7 +7541,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B38" t="s">
         <v>187</v>
@@ -7244,7 +7550,7 @@
         <v>0.9</v>
       </c>
       <c r="D38" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -7255,7 +7561,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B39" t="s">
         <v>187</v>
@@ -7264,7 +7570,7 @@
         <v>0.9</v>
       </c>
       <c r="D39" s="64" t="s">
-        <v>194</v>
+        <v>343</v>
       </c>
       <c r="E39">
         <v>2</v>
@@ -7275,7 +7581,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B40" t="s">
         <v>187</v>
@@ -7284,7 +7590,7 @@
         <v>0.9</v>
       </c>
       <c r="D40" s="64" t="s">
-        <v>189</v>
+        <v>342</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -7295,7 +7601,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B41" t="s">
         <v>187</v>
@@ -7315,7 +7621,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B42" t="s">
         <v>187</v>
@@ -7324,7 +7630,7 @@
         <v>0.9</v>
       </c>
       <c r="D42" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E42">
         <v>3</v>
@@ -7335,7 +7641,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B43" t="s">
         <v>187</v>
@@ -7344,7 +7650,7 @@
         <v>0.9</v>
       </c>
       <c r="D43" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E43">
         <v>3</v>
@@ -7355,7 +7661,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B44" t="s">
         <v>187</v>
@@ -7364,7 +7670,7 @@
         <v>0.9</v>
       </c>
       <c r="D44" s="64" t="s">
-        <v>194</v>
+        <v>343</v>
       </c>
       <c r="E44">
         <v>3</v>
@@ -7375,7 +7681,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B45" t="s">
         <v>187</v>
@@ -7384,7 +7690,7 @@
         <v>0.9</v>
       </c>
       <c r="D45" s="64" t="s">
-        <v>189</v>
+        <v>342</v>
       </c>
       <c r="E45">
         <v>3</v>
@@ -7395,7 +7701,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B46" t="s">
         <v>187</v>
@@ -7415,7 +7721,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B47" t="s">
         <v>187</v>
@@ -7424,7 +7730,7 @@
         <v>0.9</v>
       </c>
       <c r="D47" s="64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E47">
         <v>4</v>
@@ -7435,7 +7741,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B48" t="s">
         <v>187</v>
@@ -7444,7 +7750,7 @@
         <v>0.9</v>
       </c>
       <c r="D48" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E48">
         <v>4</v>
@@ -7455,7 +7761,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B49" t="s">
         <v>187</v>
@@ -7464,7 +7770,7 @@
         <v>0.9</v>
       </c>
       <c r="D49" s="64" t="s">
-        <v>194</v>
+        <v>343</v>
       </c>
       <c r="E49">
         <v>4</v>
@@ -7475,7 +7781,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B50" t="s">
         <v>187</v>
@@ -7484,7 +7790,7 @@
         <v>0.9</v>
       </c>
       <c r="D50" s="64" t="s">
-        <v>189</v>
+        <v>342</v>
       </c>
       <c r="E50">
         <v>4</v>
@@ -7495,7 +7801,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B51" t="s">
         <v>187</v>
@@ -7511,6 +7817,2006 @@
       </c>
       <c r="F51">
         <v>3.7815655654191802E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>240</v>
+      </c>
+      <c r="B52" t="s">
+        <v>241</v>
+      </c>
+      <c r="C52" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>3.5925555804288398E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>242</v>
+      </c>
+      <c r="B53" t="s">
+        <v>241</v>
+      </c>
+      <c r="C53" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>342</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>4.4994586829736297E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>243</v>
+      </c>
+      <c r="B54" t="s">
+        <v>241</v>
+      </c>
+      <c r="C54" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>190</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>4.28818435468349E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>244</v>
+      </c>
+      <c r="B55" t="s">
+        <v>241</v>
+      </c>
+      <c r="C55" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>343</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>3.8860577509801E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>245</v>
+      </c>
+      <c r="B56" t="s">
+        <v>241</v>
+      </c>
+      <c r="C56" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>194</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>3.7840391369862197E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>246</v>
+      </c>
+      <c r="B57" t="s">
+        <v>241</v>
+      </c>
+      <c r="C57" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>6.74876358965905E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>247</v>
+      </c>
+      <c r="B58" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D58" t="s">
+        <v>342</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>3.8781553903764497E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>249</v>
+      </c>
+      <c r="B59" t="s">
+        <v>248</v>
+      </c>
+      <c r="C59" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D59" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>2.1832871581523899E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>250</v>
+      </c>
+      <c r="B60" t="s">
+        <v>248</v>
+      </c>
+      <c r="C60" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D60" t="s">
+        <v>190</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>2.7664578095524899E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>251</v>
+      </c>
+      <c r="B61" t="s">
+        <v>248</v>
+      </c>
+      <c r="C61" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>343</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>2.1265061555391099E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>252</v>
+      </c>
+      <c r="B62" t="s">
+        <v>248</v>
+      </c>
+      <c r="C62" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>194</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>2.3175318601504399E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>253</v>
+      </c>
+      <c r="B63" t="s">
+        <v>241</v>
+      </c>
+      <c r="C63" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>4.9669733327683797E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>254</v>
+      </c>
+      <c r="B64" t="s">
+        <v>241</v>
+      </c>
+      <c r="C64" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D64" t="s">
+        <v>342</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>3.6503881482332398E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>255</v>
+      </c>
+      <c r="B65" t="s">
+        <v>241</v>
+      </c>
+      <c r="C65" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D65" t="s">
+        <v>194</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>3.9933582592130999E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>256</v>
+      </c>
+      <c r="B66" t="s">
+        <v>241</v>
+      </c>
+      <c r="C66" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D66" t="s">
+        <v>343</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>2.33906239966057E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>257</v>
+      </c>
+      <c r="B67" t="s">
+        <v>241</v>
+      </c>
+      <c r="C67" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D67" t="s">
+        <v>78</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>1.8611857686878501E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>258</v>
+      </c>
+      <c r="B68" t="s">
+        <v>241</v>
+      </c>
+      <c r="C68" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D68" t="s">
+        <v>190</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>3.9338671343750999E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>259</v>
+      </c>
+      <c r="B69" t="s">
+        <v>241</v>
+      </c>
+      <c r="C69" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D69" t="s">
+        <v>343</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>3.5094177612809099E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>260</v>
+      </c>
+      <c r="B70" t="s">
+        <v>241</v>
+      </c>
+      <c r="C70" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D70" t="s">
+        <v>342</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>4.6893188430530502E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>261</v>
+      </c>
+      <c r="B71" t="s">
+        <v>241</v>
+      </c>
+      <c r="C71" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>194</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>4.0537973366087603E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>262</v>
+      </c>
+      <c r="B72" t="s">
+        <v>248</v>
+      </c>
+      <c r="C72" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D72" t="s">
+        <v>342</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>3.7124207107276298E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>263</v>
+      </c>
+      <c r="B73" t="s">
+        <v>248</v>
+      </c>
+      <c r="C73" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>78</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>2.2979687803278699E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>264</v>
+      </c>
+      <c r="B74" t="s">
+        <v>241</v>
+      </c>
+      <c r="C74" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D74" t="s">
+        <v>78</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="F74">
+        <v>3.2478176652951399E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>265</v>
+      </c>
+      <c r="B75" t="s">
+        <v>248</v>
+      </c>
+      <c r="C75" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D75" t="s">
+        <v>190</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>2.8070362024871998E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>266</v>
+      </c>
+      <c r="B76" t="s">
+        <v>248</v>
+      </c>
+      <c r="C76" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D76" t="s">
+        <v>343</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>2.1116949690460799E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>267</v>
+      </c>
+      <c r="B77" t="s">
+        <v>248</v>
+      </c>
+      <c r="C77" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D77" t="s">
+        <v>194</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>2.3602783056645399E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>268</v>
+      </c>
+      <c r="B78" t="s">
+        <v>241</v>
+      </c>
+      <c r="C78" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D78" t="s">
+        <v>190</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>2.7898596235044999E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>269</v>
+      </c>
+      <c r="B79" t="s">
+        <v>248</v>
+      </c>
+      <c r="C79" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D79" t="s">
+        <v>78</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>1.6269230214792998E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>341</v>
+      </c>
+      <c r="B80" t="s">
+        <v>248</v>
+      </c>
+      <c r="C80" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D80" t="s">
+        <v>342</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>1.4296613746847601E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>340</v>
+      </c>
+      <c r="B81" t="s">
+        <v>248</v>
+      </c>
+      <c r="C81" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D81" t="s">
+        <v>190</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>2.3228051037094799E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>339</v>
+      </c>
+      <c r="B82" t="s">
+        <v>248</v>
+      </c>
+      <c r="C82" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D82" t="s">
+        <v>194</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>2.6060984472917E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>338</v>
+      </c>
+      <c r="B83" t="s">
+        <v>248</v>
+      </c>
+      <c r="C83" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D83" t="s">
+        <v>343</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>2.1548896641557898E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>337</v>
+      </c>
+      <c r="B84" t="s">
+        <v>241</v>
+      </c>
+      <c r="C84" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D84" t="s">
+        <v>194</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>2.49721747882189E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>336</v>
+      </c>
+      <c r="B85" t="s">
+        <v>241</v>
+      </c>
+      <c r="C85" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D85" t="s">
+        <v>343</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>2.8339652499992998E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>335</v>
+      </c>
+      <c r="B86" t="s">
+        <v>241</v>
+      </c>
+      <c r="C86" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D86" t="s">
+        <v>342</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>2.7059525714546201E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>334</v>
+      </c>
+      <c r="B87" t="s">
+        <v>241</v>
+      </c>
+      <c r="C87" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D87" t="s">
+        <v>78</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>2.20248632579657E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>333</v>
+      </c>
+      <c r="B88" t="s">
+        <v>241</v>
+      </c>
+      <c r="C88" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D88" t="s">
+        <v>190</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88">
+        <v>4.3232423188944297E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>332</v>
+      </c>
+      <c r="B89" t="s">
+        <v>241</v>
+      </c>
+      <c r="C89" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D89" t="s">
+        <v>343</v>
+      </c>
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="F89">
+        <v>4.5742936404417602E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>331</v>
+      </c>
+      <c r="B90" t="s">
+        <v>241</v>
+      </c>
+      <c r="C90" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D90" t="s">
+        <v>342</v>
+      </c>
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="F90">
+        <v>4.5412012525313898E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>330</v>
+      </c>
+      <c r="B91" t="s">
+        <v>241</v>
+      </c>
+      <c r="C91" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>194</v>
+      </c>
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="F91">
+        <v>3.0389519238268201E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>329</v>
+      </c>
+      <c r="B92" t="s">
+        <v>248</v>
+      </c>
+      <c r="C92" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D92" t="s">
+        <v>342</v>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92">
+        <v>3.6962289988285997E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>328</v>
+      </c>
+      <c r="B93" t="s">
+        <v>248</v>
+      </c>
+      <c r="C93" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D93" t="s">
+        <v>78</v>
+      </c>
+      <c r="E93">
+        <v>2</v>
+      </c>
+      <c r="F93">
+        <v>2.30104692992661E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>327</v>
+      </c>
+      <c r="B94" t="s">
+        <v>241</v>
+      </c>
+      <c r="C94" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D94" t="s">
+        <v>190</v>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94">
+        <v>5.2074030093785799E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>326</v>
+      </c>
+      <c r="B95" t="s">
+        <v>248</v>
+      </c>
+      <c r="C95" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D95" t="s">
+        <v>342</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>1.6472500163638298E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>325</v>
+      </c>
+      <c r="B96" t="s">
+        <v>248</v>
+      </c>
+      <c r="C96" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D96" t="s">
+        <v>190</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96">
+        <v>2.8687002464046402E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>324</v>
+      </c>
+      <c r="B97" t="s">
+        <v>248</v>
+      </c>
+      <c r="C97" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D97" t="s">
+        <v>190</v>
+      </c>
+      <c r="E97">
+        <v>2</v>
+      </c>
+      <c r="F97">
+        <v>2.6016419502468999E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>323</v>
+      </c>
+      <c r="B98" t="s">
+        <v>248</v>
+      </c>
+      <c r="C98" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D98" t="s">
+        <v>343</v>
+      </c>
+      <c r="E98">
+        <v>2</v>
+      </c>
+      <c r="F98">
+        <v>2.1379666285805801E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>322</v>
+      </c>
+      <c r="B99" t="s">
+        <v>248</v>
+      </c>
+      <c r="C99" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D99" t="s">
+        <v>78</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>2.0095605595213201E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>321</v>
+      </c>
+      <c r="B100" t="s">
+        <v>248</v>
+      </c>
+      <c r="C100" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D100" t="s">
+        <v>194</v>
+      </c>
+      <c r="E100">
+        <v>2</v>
+      </c>
+      <c r="F100">
+        <v>2.2527680424273701E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>320</v>
+      </c>
+      <c r="B101" t="s">
+        <v>248</v>
+      </c>
+      <c r="C101" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D101" t="s">
+        <v>343</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>2.3975866680038399E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>319</v>
+      </c>
+      <c r="B102" t="s">
+        <v>248</v>
+      </c>
+      <c r="C102" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D102" t="s">
+        <v>194</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>1.91012864931836E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>318</v>
+      </c>
+      <c r="B103" t="s">
+        <v>241</v>
+      </c>
+      <c r="C103" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D103" t="s">
+        <v>194</v>
+      </c>
+      <c r="E103">
+        <v>2</v>
+      </c>
+      <c r="F103">
+        <v>2.1019678834062801E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>317</v>
+      </c>
+      <c r="B104" t="s">
+        <v>241</v>
+      </c>
+      <c r="C104" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>78</v>
+      </c>
+      <c r="E104">
+        <v>3</v>
+      </c>
+      <c r="F104">
+        <v>5.46887164466274E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>316</v>
+      </c>
+      <c r="B105" t="s">
+        <v>241</v>
+      </c>
+      <c r="C105" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D105" t="s">
+        <v>343</v>
+      </c>
+      <c r="E105">
+        <v>2</v>
+      </c>
+      <c r="F105">
+        <v>3.00184733101432E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>315</v>
+      </c>
+      <c r="B106" t="s">
+        <v>241</v>
+      </c>
+      <c r="C106" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D106" t="s">
+        <v>342</v>
+      </c>
+      <c r="E106">
+        <v>2</v>
+      </c>
+      <c r="F106">
+        <v>5.6181216915425998E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>314</v>
+      </c>
+      <c r="B107" t="s">
+        <v>241</v>
+      </c>
+      <c r="C107" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D107" t="s">
+        <v>78</v>
+      </c>
+      <c r="E107">
+        <v>2</v>
+      </c>
+      <c r="F107">
+        <v>3.4828921414480699E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>313</v>
+      </c>
+      <c r="B108" t="s">
+        <v>241</v>
+      </c>
+      <c r="C108" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D108" t="s">
+        <v>190</v>
+      </c>
+      <c r="E108">
+        <v>3</v>
+      </c>
+      <c r="F108">
+        <v>5.3917054149708599E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>312</v>
+      </c>
+      <c r="B109" t="s">
+        <v>248</v>
+      </c>
+      <c r="C109" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D109" t="s">
+        <v>78</v>
+      </c>
+      <c r="E109">
+        <v>2</v>
+      </c>
+      <c r="F109">
+        <v>2.02512903086993E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>311</v>
+      </c>
+      <c r="B110" t="s">
+        <v>248</v>
+      </c>
+      <c r="C110" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D110" t="s">
+        <v>190</v>
+      </c>
+      <c r="E110">
+        <v>2</v>
+      </c>
+      <c r="F110">
+        <v>2.1056249125863E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>310</v>
+      </c>
+      <c r="B111" t="s">
+        <v>248</v>
+      </c>
+      <c r="C111" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D111" t="s">
+        <v>342</v>
+      </c>
+      <c r="E111">
+        <v>2</v>
+      </c>
+      <c r="F111">
+        <v>1.09918310194382E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>309</v>
+      </c>
+      <c r="B112" t="s">
+        <v>248</v>
+      </c>
+      <c r="C112" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D112" t="s">
+        <v>194</v>
+      </c>
+      <c r="E112">
+        <v>2</v>
+      </c>
+      <c r="F112">
+        <v>2.7731385045183202E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>308</v>
+      </c>
+      <c r="B113" t="s">
+        <v>248</v>
+      </c>
+      <c r="C113" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D113" t="s">
+        <v>343</v>
+      </c>
+      <c r="E113">
+        <v>2</v>
+      </c>
+      <c r="F113">
+        <v>2.7136183892555399E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>307</v>
+      </c>
+      <c r="B114" t="s">
+        <v>241</v>
+      </c>
+      <c r="C114" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D114" t="s">
+        <v>190</v>
+      </c>
+      <c r="E114">
+        <v>3</v>
+      </c>
+      <c r="F114">
+        <v>4.3504924066784703E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>306</v>
+      </c>
+      <c r="B115" t="s">
+        <v>241</v>
+      </c>
+      <c r="C115" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D115" t="s">
+        <v>343</v>
+      </c>
+      <c r="E115">
+        <v>3</v>
+      </c>
+      <c r="F115">
+        <v>3.8337364924015599E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>305</v>
+      </c>
+      <c r="B116" t="s">
+        <v>241</v>
+      </c>
+      <c r="C116" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D116" t="s">
+        <v>342</v>
+      </c>
+      <c r="E116">
+        <v>3</v>
+      </c>
+      <c r="F116">
+        <v>4.3320120062488802E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>304</v>
+      </c>
+      <c r="B117" t="s">
+        <v>241</v>
+      </c>
+      <c r="C117" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D117" t="s">
+        <v>194</v>
+      </c>
+      <c r="E117">
+        <v>3</v>
+      </c>
+      <c r="F117">
+        <v>4.12190315775052E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>303</v>
+      </c>
+      <c r="B118" t="s">
+        <v>248</v>
+      </c>
+      <c r="C118" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D118" t="s">
+        <v>342</v>
+      </c>
+      <c r="E118">
+        <v>3</v>
+      </c>
+      <c r="F118">
+        <v>3.4788474244807598E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>302</v>
+      </c>
+      <c r="B119" t="s">
+        <v>248</v>
+      </c>
+      <c r="C119" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D119" t="s">
+        <v>78</v>
+      </c>
+      <c r="E119">
+        <v>3</v>
+      </c>
+      <c r="F119">
+        <v>2.2207193943223999E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>301</v>
+      </c>
+      <c r="B120" t="s">
+        <v>241</v>
+      </c>
+      <c r="C120" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D120" t="s">
+        <v>194</v>
+      </c>
+      <c r="E120">
+        <v>3</v>
+      </c>
+      <c r="F120">
+        <v>4.5037575811337598E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>300</v>
+      </c>
+      <c r="B121" t="s">
+        <v>241</v>
+      </c>
+      <c r="C121" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D121" t="s">
+        <v>342</v>
+      </c>
+      <c r="E121">
+        <v>3</v>
+      </c>
+      <c r="F121">
+        <v>5.3394737919248002E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>299</v>
+      </c>
+      <c r="B122" t="s">
+        <v>241</v>
+      </c>
+      <c r="C122" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D122" t="s">
+        <v>343</v>
+      </c>
+      <c r="E122">
+        <v>3</v>
+      </c>
+      <c r="F122">
+        <v>4.1039368071153902E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>298</v>
+      </c>
+      <c r="B123" t="s">
+        <v>248</v>
+      </c>
+      <c r="C123" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D123" t="s">
+        <v>194</v>
+      </c>
+      <c r="E123">
+        <v>3</v>
+      </c>
+      <c r="F123">
+        <v>2.2911824574976501E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>297</v>
+      </c>
+      <c r="B124" t="s">
+        <v>248</v>
+      </c>
+      <c r="C124" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D124" t="s">
+        <v>343</v>
+      </c>
+      <c r="E124">
+        <v>3</v>
+      </c>
+      <c r="F124">
+        <v>2.1551203653860301E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>296</v>
+      </c>
+      <c r="B125" t="s">
+        <v>248</v>
+      </c>
+      <c r="C125" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D125" t="s">
+        <v>190</v>
+      </c>
+      <c r="E125">
+        <v>3</v>
+      </c>
+      <c r="F125">
+        <v>2.86639597414684E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>295</v>
+      </c>
+      <c r="B126" t="s">
+        <v>241</v>
+      </c>
+      <c r="C126" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D126" t="s">
+        <v>78</v>
+      </c>
+      <c r="E126">
+        <v>4</v>
+      </c>
+      <c r="F126">
+        <v>4.4822485646439897E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>294</v>
+      </c>
+      <c r="B127" t="s">
+        <v>248</v>
+      </c>
+      <c r="C127" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D127" t="s">
+        <v>342</v>
+      </c>
+      <c r="E127">
+        <v>3</v>
+      </c>
+      <c r="F127">
+        <v>1.4978096011975001E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>293</v>
+      </c>
+      <c r="B128" t="s">
+        <v>248</v>
+      </c>
+      <c r="C128" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D128" t="s">
+        <v>190</v>
+      </c>
+      <c r="E128">
+        <v>3</v>
+      </c>
+      <c r="F128">
+        <v>2.3719839810667401E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>292</v>
+      </c>
+      <c r="B129" t="s">
+        <v>248</v>
+      </c>
+      <c r="C129" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D129" t="s">
+        <v>343</v>
+      </c>
+      <c r="E129">
+        <v>3</v>
+      </c>
+      <c r="F129">
+        <v>1.9058904857432599E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>291</v>
+      </c>
+      <c r="B130" t="s">
+        <v>248</v>
+      </c>
+      <c r="C130" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D130" t="s">
+        <v>78</v>
+      </c>
+      <c r="E130">
+        <v>3</v>
+      </c>
+      <c r="F130">
+        <v>2.8945655718400701E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>290</v>
+      </c>
+      <c r="B131" t="s">
+        <v>248</v>
+      </c>
+      <c r="C131" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D131" t="s">
+        <v>194</v>
+      </c>
+      <c r="E131">
+        <v>3</v>
+      </c>
+      <c r="F131">
+        <v>2.07632811261458E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>289</v>
+      </c>
+      <c r="B132" t="s">
+        <v>241</v>
+      </c>
+      <c r="C132" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D132" t="s">
+        <v>190</v>
+      </c>
+      <c r="E132">
+        <v>4</v>
+      </c>
+      <c r="F132">
+        <v>4.3405396749869297E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>288</v>
+      </c>
+      <c r="B133" t="s">
+        <v>241</v>
+      </c>
+      <c r="C133" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D133" t="s">
+        <v>78</v>
+      </c>
+      <c r="E133">
+        <v>3</v>
+      </c>
+      <c r="F133">
+        <v>3.7795469869662597E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>287</v>
+      </c>
+      <c r="B134" t="s">
+        <v>241</v>
+      </c>
+      <c r="C134" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D134" t="s">
+        <v>194</v>
+      </c>
+      <c r="E134">
+        <v>4</v>
+      </c>
+      <c r="F134">
+        <v>3.79338388532263E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>286</v>
+      </c>
+      <c r="B135" t="s">
+        <v>241</v>
+      </c>
+      <c r="C135" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D135" t="s">
+        <v>342</v>
+      </c>
+      <c r="E135">
+        <v>4</v>
+      </c>
+      <c r="F135">
+        <v>4.2040028674091998E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>285</v>
+      </c>
+      <c r="B136" t="s">
+        <v>241</v>
+      </c>
+      <c r="C136" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D136" t="s">
+        <v>343</v>
+      </c>
+      <c r="E136">
+        <v>4</v>
+      </c>
+      <c r="F136">
+        <v>3.5338155130564999E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>284</v>
+      </c>
+      <c r="B137" t="s">
+        <v>241</v>
+      </c>
+      <c r="C137" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D137" t="s">
+        <v>190</v>
+      </c>
+      <c r="E137">
+        <v>4</v>
+      </c>
+      <c r="F137">
+        <v>3.3946550145984702E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>283</v>
+      </c>
+      <c r="B138" t="s">
+        <v>241</v>
+      </c>
+      <c r="C138" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D138" t="s">
+        <v>342</v>
+      </c>
+      <c r="E138">
+        <v>4</v>
+      </c>
+      <c r="F138">
+        <v>4.7472359964314502E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>282</v>
+      </c>
+      <c r="B139" t="s">
+        <v>241</v>
+      </c>
+      <c r="C139" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D139" t="s">
+        <v>343</v>
+      </c>
+      <c r="E139">
+        <v>4</v>
+      </c>
+      <c r="F139">
+        <v>3.82142538177173E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>281</v>
+      </c>
+      <c r="B140" t="s">
+        <v>248</v>
+      </c>
+      <c r="C140" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D140" t="s">
+        <v>342</v>
+      </c>
+      <c r="E140">
+        <v>4</v>
+      </c>
+      <c r="F140">
+        <v>3.9192116130389698E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>280</v>
+      </c>
+      <c r="B141" t="s">
+        <v>248</v>
+      </c>
+      <c r="C141" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D141" t="s">
+        <v>78</v>
+      </c>
+      <c r="E141">
+        <v>4</v>
+      </c>
+      <c r="F141">
+        <v>2.2984341174385501E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>279</v>
+      </c>
+      <c r="B142" t="s">
+        <v>241</v>
+      </c>
+      <c r="C142" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D142" t="s">
+        <v>194</v>
+      </c>
+      <c r="E142">
+        <v>4</v>
+      </c>
+      <c r="F142">
+        <v>2.99967104119803E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>278</v>
+      </c>
+      <c r="B143" t="s">
+        <v>248</v>
+      </c>
+      <c r="C143" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D143" t="s">
+        <v>194</v>
+      </c>
+      <c r="E143">
+        <v>4</v>
+      </c>
+      <c r="F143">
+        <v>2.24512265915131E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>277</v>
+      </c>
+      <c r="B144" t="s">
+        <v>248</v>
+      </c>
+      <c r="C144" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D144" t="s">
+        <v>190</v>
+      </c>
+      <c r="E144">
+        <v>4</v>
+      </c>
+      <c r="F144">
+        <v>2.76438284773496E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>276</v>
+      </c>
+      <c r="B145" t="s">
+        <v>248</v>
+      </c>
+      <c r="C145" s="66">
+        <v>0.9</v>
+      </c>
+      <c r="D145" t="s">
+        <v>343</v>
+      </c>
+      <c r="E145">
+        <v>4</v>
+      </c>
+      <c r="F145">
+        <v>2.1253487733380601E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>275</v>
+      </c>
+      <c r="B146" t="s">
+        <v>248</v>
+      </c>
+      <c r="C146" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D146" t="s">
+        <v>343</v>
+      </c>
+      <c r="E146">
+        <v>4</v>
+      </c>
+      <c r="F146">
+        <v>1.8628456891274899E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>274</v>
+      </c>
+      <c r="B147" t="s">
+        <v>248</v>
+      </c>
+      <c r="C147" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D147" t="s">
+        <v>194</v>
+      </c>
+      <c r="E147">
+        <v>4</v>
+      </c>
+      <c r="F147">
+        <v>2.1588098071542199E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>273</v>
+      </c>
+      <c r="B148" t="s">
+        <v>248</v>
+      </c>
+      <c r="C148" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D148" t="s">
+        <v>190</v>
+      </c>
+      <c r="E148">
+        <v>4</v>
+      </c>
+      <c r="F148">
+        <v>2.0395442160772499E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>272</v>
+      </c>
+      <c r="B149" t="s">
+        <v>248</v>
+      </c>
+      <c r="C149" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D149" t="s">
+        <v>342</v>
+      </c>
+      <c r="E149">
+        <v>4</v>
+      </c>
+      <c r="F149">
+        <v>1.76568131244636E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>271</v>
+      </c>
+      <c r="B150" t="s">
+        <v>248</v>
+      </c>
+      <c r="C150" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D150" t="s">
+        <v>78</v>
+      </c>
+      <c r="E150">
+        <v>4</v>
+      </c>
+      <c r="F150">
+        <v>2.0008016010584499E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>270</v>
+      </c>
+      <c r="B151" t="s">
+        <v>241</v>
+      </c>
+      <c r="C151" s="66">
+        <v>0.33</v>
+      </c>
+      <c r="D151" t="s">
+        <v>78</v>
+      </c>
+      <c r="E151">
+        <v>4</v>
+      </c>
+      <c r="F151">
+        <v>2.35711201484251E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>